<commit_message>
escenarios de caso de uso: ABM personal y ABM usuario
</commit_message>
<xml_diff>
--- a/editECU/Alta usuario.xlsx
+++ b/editECU/Alta usuario.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Escenario de Caso de Uso" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Nombre del Caso de Uso:</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Riesgo:</t>
   </si>
   <si>
-    <t>Alta usuario</t>
-  </si>
-  <si>
     <t>ID única: 001</t>
   </si>
   <si>
@@ -99,15 +96,9 @@
     <t>Registro en la base de datos de SUGPA</t>
   </si>
   <si>
-    <t>Permite instanciar nuevos usuarios en el sistema según se requieran</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
-    <t>Tabla 1 Escenario de Caso de Uso 1</t>
-  </si>
-  <si>
     <t>Externa</t>
   </si>
   <si>
@@ -115,6 +106,12 @@
   </si>
   <si>
     <t>Asigna un ID de forma automática, el Usuario es el email y la Contraseña es el dni</t>
+  </si>
+  <si>
+    <t>Alta Usuario</t>
+  </si>
+  <si>
+    <t>Permite instanciar nuevos usuarios en el sistema, según se requiera</t>
   </si>
 </sst>
 </file>
@@ -151,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -211,20 +208,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,13 +224,34 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,21 +261,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,189 +544,183 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" ht="33" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" ht="33" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="33" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="33" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" ht="33" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:4" ht="23.25" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" ht="21.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:4" ht="24.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="31.5" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:4" ht="24" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="22.95" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" ht="31.5" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4" ht="45" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:4" ht="32.25" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-    </row>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>

</xml_diff>